<commit_message>
Updated Excel file via Streamlit
</commit_message>
<xml_diff>
--- a/Generated_Responses.xlsx
+++ b/Generated_Responses.xlsx
@@ -22,61 +22,61 @@
     <t>What is the membership count for society_name? Respond with one word (number) only. That should just be an integer nothing like approx or members just a number.</t>
   </si>
   <si>
-    <t>"Does society_name encompasses community sites? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma."</t>
-  </si>
-  <si>
-    <t>"Is society_name influential on state or local policy? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma."</t>
-  </si>
-  <si>
-    <t>"Does society_name provide engagement opportunity with leadership? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma."</t>
-  </si>
-  <si>
-    <t>"Does society_name provide support for clinical trial recruitment? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma."</t>
-  </si>
-  <si>
-    <t>"Does society_name provide engagement opportunity with payors? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma."</t>
-  </si>
-  <si>
-    <t>"Does society_name include area experts on its board? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma."</t>
-  </si>
-  <si>
-    <t>"Is society_name involved in therapeutic research collaborations? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.",</t>
-  </si>
-  <si>
-    <t>"Does society_name include top therapeutic area experts on its board? Respond with one word ('yes' or 'no') only plus provide a justification for the answer also after a comma."</t>
-  </si>
-  <si>
-    <t>"Name the Region where the society_name is from? Just name the US state or the Region in one word for the answer."</t>
+    <t>Does society_name encompasses community sites? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.</t>
+  </si>
+  <si>
+    <t>Is society_name influential on state or local policy? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.</t>
+  </si>
+  <si>
+    <t>Does society_name provide engagement opportunity with leadership? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.</t>
+  </si>
+  <si>
+    <t>Does society_name provide support for clinical trial recruitment? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.</t>
+  </si>
+  <si>
+    <t>Does society_name provide engagement opportunity with payors? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.</t>
+  </si>
+  <si>
+    <t>Does society_name include area experts on its board? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.</t>
+  </si>
+  <si>
+    <t>Is society_name involved in therapeutic research collaborations? Respond one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.</t>
+  </si>
+  <si>
+    <t>Does society_name include top therapeutic area experts on its board? Respond with one word ('yes' or 'no') only plus provide a justification for the answer also after a comma.</t>
+  </si>
+  <si>
+    <t>Name the Region where the society_name is from? Just name the US state or the Region in one word for the answer.</t>
   </si>
   <si>
     <t>Soleo Health</t>
   </si>
   <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>No, Soleo Health does not encompass community sites. Soleo Health is a specialty pharmacy focused on providing IV and injectable medications directly to patients' homes, rather than operating community sites for public engagement or support.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health is not influential on state or local policy. The society is primarily focused on providing healthcare services rather than engaging in policy advocacy or lobbying.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health does not provide engagement opportunity with leadership. The company focuses more on patient care and healthcare services rather than direct engagement with leadership.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health, the society named, does not provide support for clinical trial recruitment. Soleo Health focuses on specialty infusion services rather than clinical trial recruitment.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health does not provide engagement opportunity with payors. Soleo Health is a specialty infusion provider focusing on patient care services and does not actively engage with payors for business purposes.</t>
-  </si>
-  <si>
-    <t>Yes, Soleo Health does include area experts on its board. Having area experts on the board brings diverse perspectives and specialized knowledge to the organization's decision-making processes.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health is not involved in therapeutic research collaborations. Soleo Health is a specialty pharmacy focused on providing high-quality infusion therapy services rather than engaging in research collaborations.</t>
-  </si>
-  <si>
-    <t>No, justification: Soleo Health does not include top therapeutic area experts on its board.</t>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>No, Soleo Health does not encompass community sites. Soleo Health is a specialty infusion pharmacy providing services to patients in their homes or at infusion suites.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health is not influential on state or local policy. The society's focus is on providing healthcare services rather than direct involvement in policy-making.</t>
+  </si>
+  <si>
+    <t>Yes, Soleo Health provides engagement opportunity with leadership. The company emphasizes connecting with and involving employees at all levels to foster communication and collaboration.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health does not provide support for clinical trial recruitment. Soleo Health is a specialty pharmacy that focuses on providing infusion therapy services rather than clinical trial support.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health does not engage with payors. They focus on providing specialized pharmacy services directly to patients and healthcare providers.</t>
+  </si>
+  <si>
+    <t>Yes, Soleo Health includes area experts on its board. This is important for bringing diverse perspectives and specialized knowledge to the decision-making process.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health is not involved in therapeutic research collaborations. Justification: Soleo Health focuses on providing specialized pharmacy and nursing services to patients with complex and chronic conditions, rather than conducting research collaborations.</t>
+  </si>
+  <si>
+    <t>No, justification: No information publicly available regarding the expertise of the board members at Soleo Health in specific therapeutic areas.</t>
   </si>
   <si>
     <t>Texas</t>

</xml_diff>